<commit_message>
Tidy and organisation of various files. Notable addition of the minimum investments email generator for FM Admin use.
</commit_message>
<xml_diff>
--- a/AOL/Fund_List_V4.xlsx
+++ b/AOL/Fund_List_V4.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RArm1\PycharmProjects\Account Opening Letter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Fund Management\Fund Management Team Files\FM Personal Folders\Richard\PycharmProjects\AOL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFD686AD-E262-4742-B0C4-911DCBEE529D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9832B0B7-E7B3-4E9C-B5C9-50FA0181CF2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D942DA33-F7AF-44DF-9B00-6E371688402A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D942DA33-F7AF-44DF-9B00-6E371688402A}"/>
   </bookViews>
   <sheets>
     <sheet name="Fund List" sheetId="1" r:id="rId1"/>
@@ -259,37 +259,37 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -609,7 +609,7 @@
   <dimension ref="A1:K42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="A5:XFD16"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -749,500 +749,540 @@
       <c r="K5" s="13"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="20"/>
-      <c r="B6" s="21"/>
-      <c r="C6" s="22"/>
+      <c r="A6" s="23"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="29"/>
       <c r="D6" s="1"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
       <c r="I6" s="19"/>
       <c r="J6" s="19"/>
       <c r="K6" s="19"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="20"/>
-      <c r="B7" s="21"/>
-      <c r="C7" s="22"/>
+      <c r="A7" s="23"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="29"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
       <c r="I7" s="19"/>
       <c r="J7" s="19"/>
       <c r="K7" s="19"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="20"/>
-      <c r="B8" s="21"/>
-      <c r="C8" s="22"/>
+      <c r="A8" s="23"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="29"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
       <c r="I8" s="19"/>
       <c r="J8" s="19"/>
       <c r="K8" s="19"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="20"/>
-      <c r="B9" s="21"/>
-      <c r="C9" s="22"/>
+      <c r="A9" s="23"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="29"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
       <c r="I9" s="19"/>
       <c r="J9" s="19"/>
       <c r="K9" s="19"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="20"/>
-      <c r="B10" s="21"/>
-      <c r="C10" s="22"/>
+      <c r="A10" s="23"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="29"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="23"/>
       <c r="I10" s="19"/>
       <c r="J10" s="19"/>
       <c r="K10" s="19"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="20"/>
-      <c r="B11" s="21"/>
-      <c r="C11" s="22"/>
+      <c r="A11" s="23"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="29"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="23"/>
       <c r="I11" s="19"/>
       <c r="J11" s="19"/>
       <c r="K11" s="19"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="20"/>
-      <c r="B12" s="21"/>
-      <c r="C12" s="22"/>
+      <c r="A12" s="23"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="29"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23"/>
       <c r="I12" s="19"/>
       <c r="J12" s="19"/>
       <c r="K12" s="19"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="20"/>
-      <c r="B13" s="21"/>
-      <c r="C13" s="22"/>
+      <c r="A13" s="23"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="29"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="23"/>
       <c r="I13" s="19"/>
       <c r="J13" s="19"/>
       <c r="K13" s="19"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="20"/>
-      <c r="B14" s="21"/>
-      <c r="C14" s="22"/>
+      <c r="A14" s="23"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="29"/>
       <c r="D14" s="1"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
       <c r="I14" s="19"/>
       <c r="J14" s="19"/>
       <c r="K14" s="19"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="20"/>
-      <c r="B15" s="21"/>
-      <c r="C15" s="22"/>
+      <c r="A15" s="23"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="29"/>
       <c r="D15" s="1"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
       <c r="I15" s="19"/>
       <c r="J15" s="19"/>
       <c r="K15" s="19"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="20"/>
-      <c r="B16" s="21"/>
-      <c r="C16" s="22"/>
+      <c r="A16" s="23"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="29"/>
       <c r="D16" s="1"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="23"/>
       <c r="I16" s="19"/>
       <c r="J16" s="19"/>
       <c r="K16" s="19"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="24"/>
-      <c r="B17" s="25"/>
-      <c r="C17" s="26"/>
+      <c r="A17" s="20"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="30"/>
       <c r="D17" s="2"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="24"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="31"/>
+      <c r="H17" s="20"/>
       <c r="I17" s="19"/>
       <c r="J17" s="19"/>
       <c r="K17" s="19"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="24"/>
-      <c r="B18" s="25"/>
-      <c r="C18" s="26"/>
+      <c r="A18" s="20"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="30"/>
       <c r="D18" s="2"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="24"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="31"/>
+      <c r="H18" s="20"/>
       <c r="I18" s="19"/>
       <c r="J18" s="19"/>
       <c r="K18" s="19"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="24"/>
-      <c r="B19" s="25"/>
-      <c r="C19" s="26"/>
+      <c r="A19" s="20"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="30"/>
       <c r="D19" s="2"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="28"/>
-      <c r="H19" s="24"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="31"/>
+      <c r="H19" s="20"/>
       <c r="I19" s="19"/>
       <c r="J19" s="19"/>
       <c r="K19" s="19"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="20"/>
-      <c r="B20" s="21"/>
-      <c r="C20" s="22"/>
+      <c r="A20" s="23"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="29"/>
       <c r="D20" s="1"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="20"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="23"/>
       <c r="I20" s="19"/>
       <c r="J20" s="19"/>
       <c r="K20" s="19"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="20"/>
-      <c r="B21" s="21"/>
-      <c r="C21" s="22"/>
+      <c r="A21" s="23"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="29"/>
       <c r="D21" s="1"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="23"/>
       <c r="I21" s="19"/>
       <c r="J21" s="19"/>
       <c r="K21" s="19"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="20"/>
-      <c r="B22" s="21"/>
-      <c r="C22" s="22"/>
+      <c r="A22" s="23"/>
+      <c r="B22" s="24"/>
+      <c r="C22" s="29"/>
       <c r="D22" s="1"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="20"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="23"/>
+      <c r="G22" s="23"/>
+      <c r="H22" s="23"/>
       <c r="I22" s="19"/>
       <c r="J22" s="19"/>
       <c r="K22" s="19"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="20"/>
-      <c r="B23" s="21"/>
-      <c r="C23" s="22"/>
+      <c r="A23" s="23"/>
+      <c r="B23" s="24"/>
+      <c r="C23" s="29"/>
       <c r="D23" s="1"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="20"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="23"/>
       <c r="I23" s="19"/>
       <c r="J23" s="19"/>
       <c r="K23" s="19"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="20"/>
-      <c r="B24" s="21"/>
-      <c r="C24" s="22"/>
+      <c r="A24" s="23"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="29"/>
       <c r="D24" s="1"/>
-      <c r="E24" s="23"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="20"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="23"/>
+      <c r="G24" s="23"/>
+      <c r="H24" s="23"/>
       <c r="I24" s="19"/>
       <c r="J24" s="19"/>
       <c r="K24" s="19"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="20"/>
-      <c r="B25" s="21"/>
-      <c r="C25" s="29"/>
+      <c r="A25" s="23"/>
+      <c r="B25" s="24"/>
+      <c r="C25" s="27"/>
       <c r="D25" s="1"/>
-      <c r="E25" s="23"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="20"/>
-      <c r="H25" s="20"/>
+      <c r="E25" s="28"/>
+      <c r="F25" s="23"/>
+      <c r="G25" s="23"/>
+      <c r="H25" s="23"/>
       <c r="I25" s="19"/>
       <c r="J25" s="19"/>
       <c r="K25" s="19"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="20"/>
-      <c r="B26" s="21"/>
-      <c r="C26" s="29"/>
+      <c r="A26" s="23"/>
+      <c r="B26" s="24"/>
+      <c r="C26" s="27"/>
       <c r="D26" s="1"/>
-      <c r="E26" s="23"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20"/>
-      <c r="H26" s="20"/>
+      <c r="E26" s="28"/>
+      <c r="F26" s="23"/>
+      <c r="G26" s="23"/>
+      <c r="H26" s="23"/>
       <c r="I26" s="19"/>
       <c r="J26" s="19"/>
       <c r="K26" s="19"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="20"/>
-      <c r="B27" s="21"/>
-      <c r="C27" s="29"/>
+      <c r="A27" s="23"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="27"/>
       <c r="D27" s="1"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="20"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="23"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="23"/>
       <c r="I27" s="19"/>
       <c r="J27" s="19"/>
       <c r="K27" s="19"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="20"/>
-      <c r="B28" s="21"/>
-      <c r="C28" s="29"/>
+      <c r="A28" s="23"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="27"/>
       <c r="D28" s="1"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="20"/>
-      <c r="G28" s="20"/>
-      <c r="H28" s="20"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="23"/>
       <c r="I28" s="19"/>
       <c r="J28" s="19"/>
       <c r="K28" s="19"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="20"/>
-      <c r="B29" s="21"/>
-      <c r="C29" s="29"/>
+      <c r="A29" s="23"/>
+      <c r="B29" s="24"/>
+      <c r="C29" s="27"/>
       <c r="D29" s="1"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="20"/>
-      <c r="G29" s="20"/>
-      <c r="H29" s="20"/>
+      <c r="E29" s="28"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="23"/>
+      <c r="H29" s="23"/>
       <c r="I29" s="19"/>
       <c r="J29" s="19"/>
       <c r="K29" s="19"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="24"/>
-      <c r="B30" s="25"/>
-      <c r="C30" s="30"/>
+      <c r="A30" s="20"/>
+      <c r="B30" s="21"/>
+      <c r="C30" s="26"/>
       <c r="D30" s="2"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="24"/>
-      <c r="G30" s="24"/>
-      <c r="H30" s="24"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
       <c r="I30" s="19"/>
       <c r="J30" s="19"/>
       <c r="K30" s="19"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="24"/>
-      <c r="B31" s="25"/>
-      <c r="C31" s="30"/>
+      <c r="A31" s="20"/>
+      <c r="B31" s="21"/>
+      <c r="C31" s="26"/>
       <c r="D31" s="2"/>
-      <c r="E31" s="27"/>
-      <c r="F31" s="24"/>
-      <c r="G31" s="24"/>
-      <c r="H31" s="24"/>
+      <c r="E31" s="22"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="20"/>
       <c r="I31" s="19"/>
       <c r="J31" s="19"/>
       <c r="K31" s="19"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="24"/>
-      <c r="B32" s="25"/>
-      <c r="C32" s="30"/>
+      <c r="A32" s="20"/>
+      <c r="B32" s="21"/>
+      <c r="C32" s="26"/>
       <c r="D32" s="2"/>
-      <c r="E32" s="27"/>
-      <c r="F32" s="24"/>
-      <c r="G32" s="24"/>
-      <c r="H32" s="24"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="20"/>
       <c r="I32" s="19"/>
       <c r="J32" s="19"/>
       <c r="K32" s="19"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="20"/>
-      <c r="B33" s="21"/>
-      <c r="C33" s="20"/>
+      <c r="A33" s="23"/>
+      <c r="B33" s="24"/>
+      <c r="C33" s="23"/>
       <c r="D33" s="1"/>
-      <c r="E33" s="31"/>
-      <c r="F33" s="20"/>
-      <c r="G33" s="20"/>
-      <c r="H33" s="20"/>
+      <c r="E33" s="25"/>
+      <c r="F33" s="23"/>
+      <c r="G33" s="23"/>
+      <c r="H33" s="23"/>
       <c r="I33" s="19"/>
       <c r="J33" s="19"/>
       <c r="K33" s="19"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="20"/>
-      <c r="B34" s="21"/>
-      <c r="C34" s="20"/>
+      <c r="A34" s="23"/>
+      <c r="B34" s="24"/>
+      <c r="C34" s="23"/>
       <c r="D34" s="1"/>
-      <c r="E34" s="31"/>
-      <c r="F34" s="20"/>
-      <c r="G34" s="20"/>
-      <c r="H34" s="20"/>
+      <c r="E34" s="25"/>
+      <c r="F34" s="23"/>
+      <c r="G34" s="23"/>
+      <c r="H34" s="23"/>
       <c r="I34" s="19"/>
       <c r="J34" s="19"/>
       <c r="K34" s="19"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="20"/>
-      <c r="B35" s="21"/>
-      <c r="C35" s="20"/>
+      <c r="A35" s="23"/>
+      <c r="B35" s="24"/>
+      <c r="C35" s="23"/>
       <c r="D35" s="1"/>
-      <c r="E35" s="31"/>
-      <c r="F35" s="20"/>
-      <c r="G35" s="20"/>
-      <c r="H35" s="20"/>
+      <c r="E35" s="25"/>
+      <c r="F35" s="23"/>
+      <c r="G35" s="23"/>
+      <c r="H35" s="23"/>
       <c r="I35" s="19"/>
       <c r="J35" s="19"/>
       <c r="K35" s="19"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="20"/>
-      <c r="B36" s="21"/>
-      <c r="C36" s="20"/>
+      <c r="A36" s="23"/>
+      <c r="B36" s="24"/>
+      <c r="C36" s="23"/>
       <c r="D36" s="1"/>
-      <c r="E36" s="31"/>
-      <c r="F36" s="20"/>
-      <c r="G36" s="20"/>
-      <c r="H36" s="20"/>
+      <c r="E36" s="25"/>
+      <c r="F36" s="23"/>
+      <c r="G36" s="23"/>
+      <c r="H36" s="23"/>
       <c r="I36" s="19"/>
       <c r="J36" s="19"/>
       <c r="K36" s="19"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="20"/>
-      <c r="B37" s="21"/>
-      <c r="C37" s="20"/>
+      <c r="A37" s="23"/>
+      <c r="B37" s="24"/>
+      <c r="C37" s="23"/>
       <c r="D37" s="1"/>
-      <c r="E37" s="31"/>
-      <c r="F37" s="20"/>
-      <c r="G37" s="20"/>
-      <c r="H37" s="20"/>
+      <c r="E37" s="25"/>
+      <c r="F37" s="23"/>
+      <c r="G37" s="23"/>
+      <c r="H37" s="23"/>
       <c r="I37" s="19"/>
       <c r="J37" s="19"/>
       <c r="K37" s="19"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="24"/>
-      <c r="B38" s="25"/>
-      <c r="C38" s="24"/>
+      <c r="A38" s="20"/>
+      <c r="B38" s="21"/>
+      <c r="C38" s="20"/>
       <c r="D38" s="3"/>
-      <c r="E38" s="27"/>
-      <c r="F38" s="24"/>
-      <c r="G38" s="24"/>
-      <c r="H38" s="24"/>
+      <c r="E38" s="22"/>
+      <c r="F38" s="20"/>
+      <c r="G38" s="20"/>
+      <c r="H38" s="20"/>
       <c r="I38" s="19"/>
       <c r="J38" s="19"/>
       <c r="K38" s="19"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="24"/>
-      <c r="B39" s="25"/>
-      <c r="C39" s="24"/>
+      <c r="A39" s="20"/>
+      <c r="B39" s="21"/>
+      <c r="C39" s="20"/>
       <c r="D39" s="3"/>
-      <c r="E39" s="27"/>
-      <c r="F39" s="24"/>
-      <c r="G39" s="24"/>
-      <c r="H39" s="24"/>
+      <c r="E39" s="22"/>
+      <c r="F39" s="20"/>
+      <c r="G39" s="20"/>
+      <c r="H39" s="20"/>
       <c r="I39" s="19"/>
       <c r="J39" s="19"/>
       <c r="K39" s="19"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="24"/>
-      <c r="B40" s="25"/>
-      <c r="C40" s="24"/>
+      <c r="A40" s="20"/>
+      <c r="B40" s="21"/>
+      <c r="C40" s="20"/>
       <c r="D40" s="3"/>
-      <c r="E40" s="27"/>
-      <c r="F40" s="24"/>
-      <c r="G40" s="24"/>
-      <c r="H40" s="24"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="20"/>
+      <c r="H40" s="20"/>
       <c r="I40" s="19"/>
       <c r="J40" s="19"/>
       <c r="K40" s="19"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="24"/>
-      <c r="B41" s="25"/>
-      <c r="C41" s="24"/>
+      <c r="A41" s="20"/>
+      <c r="B41" s="21"/>
+      <c r="C41" s="20"/>
       <c r="D41" s="3"/>
-      <c r="E41" s="27"/>
-      <c r="F41" s="24"/>
-      <c r="G41" s="24"/>
-      <c r="H41" s="24"/>
+      <c r="E41" s="22"/>
+      <c r="F41" s="20"/>
+      <c r="G41" s="20"/>
+      <c r="H41" s="20"/>
       <c r="I41" s="19"/>
       <c r="J41" s="19"/>
       <c r="K41" s="19"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="24"/>
-      <c r="B42" s="25"/>
-      <c r="C42" s="24"/>
+      <c r="A42" s="20"/>
+      <c r="B42" s="21"/>
+      <c r="C42" s="20"/>
       <c r="D42" s="3"/>
-      <c r="E42" s="27"/>
-      <c r="F42" s="24"/>
-      <c r="G42" s="24"/>
-      <c r="H42" s="24"/>
+      <c r="E42" s="22"/>
+      <c r="F42" s="20"/>
+      <c r="G42" s="20"/>
+      <c r="H42" s="20"/>
       <c r="I42" s="19"/>
       <c r="J42" s="19"/>
       <c r="K42" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="80">
-    <mergeCell ref="J38:J42"/>
-    <mergeCell ref="K38:K42"/>
-    <mergeCell ref="J33:J37"/>
-    <mergeCell ref="K33:K37"/>
-    <mergeCell ref="A38:A42"/>
-    <mergeCell ref="B38:B42"/>
-    <mergeCell ref="C38:C42"/>
-    <mergeCell ref="E38:E42"/>
-    <mergeCell ref="F38:F42"/>
-    <mergeCell ref="G38:G42"/>
-    <mergeCell ref="H38:H42"/>
-    <mergeCell ref="I38:I42"/>
+    <mergeCell ref="G6:G10"/>
+    <mergeCell ref="H6:H10"/>
+    <mergeCell ref="I6:I10"/>
+    <mergeCell ref="J6:J10"/>
+    <mergeCell ref="K6:K10"/>
+    <mergeCell ref="A6:A10"/>
+    <mergeCell ref="B6:B10"/>
+    <mergeCell ref="C6:C10"/>
+    <mergeCell ref="E6:E10"/>
+    <mergeCell ref="F6:F10"/>
+    <mergeCell ref="F11:F16"/>
+    <mergeCell ref="G11:G16"/>
+    <mergeCell ref="H11:H16"/>
+    <mergeCell ref="I11:I16"/>
+    <mergeCell ref="J11:J16"/>
+    <mergeCell ref="J20:J24"/>
+    <mergeCell ref="K11:K16"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="E17:E19"/>
+    <mergeCell ref="F17:F19"/>
+    <mergeCell ref="G17:G19"/>
+    <mergeCell ref="H17:H19"/>
+    <mergeCell ref="I17:I19"/>
+    <mergeCell ref="J17:J19"/>
+    <mergeCell ref="K17:K19"/>
+    <mergeCell ref="A11:A16"/>
+    <mergeCell ref="B11:B16"/>
+    <mergeCell ref="C11:C16"/>
+    <mergeCell ref="E11:E16"/>
+    <mergeCell ref="E20:E24"/>
+    <mergeCell ref="F20:F24"/>
+    <mergeCell ref="G20:G24"/>
+    <mergeCell ref="H20:H24"/>
+    <mergeCell ref="I20:I24"/>
+    <mergeCell ref="I30:I32"/>
+    <mergeCell ref="J30:J32"/>
+    <mergeCell ref="K20:K24"/>
+    <mergeCell ref="A25:A29"/>
+    <mergeCell ref="B25:B29"/>
+    <mergeCell ref="C25:C29"/>
+    <mergeCell ref="E25:E29"/>
+    <mergeCell ref="F25:F29"/>
+    <mergeCell ref="G25:G29"/>
+    <mergeCell ref="H25:H29"/>
+    <mergeCell ref="I25:I29"/>
+    <mergeCell ref="J25:J29"/>
+    <mergeCell ref="K25:K29"/>
+    <mergeCell ref="A20:A24"/>
+    <mergeCell ref="B20:B24"/>
+    <mergeCell ref="C20:C24"/>
     <mergeCell ref="K30:K32"/>
     <mergeCell ref="A33:A37"/>
     <mergeCell ref="B33:B37"/>
@@ -1259,58 +1299,18 @@
     <mergeCell ref="F30:F32"/>
     <mergeCell ref="G30:G32"/>
     <mergeCell ref="H30:H32"/>
-    <mergeCell ref="I30:I32"/>
-    <mergeCell ref="J30:J32"/>
-    <mergeCell ref="K20:K24"/>
-    <mergeCell ref="A25:A29"/>
-    <mergeCell ref="B25:B29"/>
-    <mergeCell ref="C25:C29"/>
-    <mergeCell ref="E25:E29"/>
-    <mergeCell ref="F25:F29"/>
-    <mergeCell ref="G25:G29"/>
-    <mergeCell ref="H25:H29"/>
-    <mergeCell ref="I25:I29"/>
-    <mergeCell ref="J25:J29"/>
-    <mergeCell ref="K25:K29"/>
-    <mergeCell ref="A20:A24"/>
-    <mergeCell ref="B20:B24"/>
-    <mergeCell ref="C20:C24"/>
-    <mergeCell ref="E20:E24"/>
-    <mergeCell ref="F20:F24"/>
-    <mergeCell ref="G20:G24"/>
-    <mergeCell ref="H20:H24"/>
-    <mergeCell ref="I20:I24"/>
-    <mergeCell ref="J20:J24"/>
-    <mergeCell ref="K11:K16"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="E17:E19"/>
-    <mergeCell ref="F17:F19"/>
-    <mergeCell ref="G17:G19"/>
-    <mergeCell ref="H17:H19"/>
-    <mergeCell ref="I17:I19"/>
-    <mergeCell ref="J17:J19"/>
-    <mergeCell ref="K17:K19"/>
-    <mergeCell ref="A11:A16"/>
-    <mergeCell ref="B11:B16"/>
-    <mergeCell ref="C11:C16"/>
-    <mergeCell ref="E11:E16"/>
-    <mergeCell ref="F11:F16"/>
-    <mergeCell ref="G11:G16"/>
-    <mergeCell ref="H11:H16"/>
-    <mergeCell ref="I11:I16"/>
-    <mergeCell ref="J11:J16"/>
-    <mergeCell ref="A6:A10"/>
-    <mergeCell ref="B6:B10"/>
-    <mergeCell ref="C6:C10"/>
-    <mergeCell ref="E6:E10"/>
-    <mergeCell ref="F6:F10"/>
-    <mergeCell ref="G6:G10"/>
-    <mergeCell ref="H6:H10"/>
-    <mergeCell ref="I6:I10"/>
-    <mergeCell ref="J6:J10"/>
-    <mergeCell ref="K6:K10"/>
+    <mergeCell ref="J38:J42"/>
+    <mergeCell ref="K38:K42"/>
+    <mergeCell ref="J33:J37"/>
+    <mergeCell ref="K33:K37"/>
+    <mergeCell ref="A38:A42"/>
+    <mergeCell ref="B38:B42"/>
+    <mergeCell ref="C38:C42"/>
+    <mergeCell ref="E38:E42"/>
+    <mergeCell ref="F38:F42"/>
+    <mergeCell ref="G38:G42"/>
+    <mergeCell ref="H38:H42"/>
+    <mergeCell ref="I38:I42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>